<commit_message>
Desenvolvendo Case Data Master - Leo
</commit_message>
<xml_diff>
--- a/pre_processing/target_encoder_city.xlsx
+++ b/pre_processing/target_encoder_city.xlsx
@@ -450,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.347</v>
+        <v>-0.326</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>0.207</v>
+        <v>0.169</v>
       </c>
     </row>
     <row r="4">
@@ -466,23 +466,23 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0.281</v>
+        <v>0.233</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.292</v>
+        <v>0.291</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>0.364</v>
+        <v>0.293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>